<commit_message>
496677 Uploading Final Version
</commit_message>
<xml_diff>
--- a/Test/IB_2_0_576 Defect Log.xlsx
+++ b/Test/IB_2_0_576 Defect Log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -67,12 +67,6 @@
     <t>3 - Minor Problem</t>
   </si>
   <si>
-    <t>IB*2.0*576T4</t>
-  </si>
-  <si>
-    <t>IB*2.0*376T4</t>
-  </si>
-  <si>
     <t>Mary Simons</t>
   </si>
   <si>
@@ -109,18 +103,12 @@
     <t>US15: Payer Zip Code Field Adjustment (USEB-1)</t>
   </si>
   <si>
-    <t>IB*2.0*576T6</t>
-  </si>
-  <si>
     <t>DE46</t>
   </si>
   <si>
     <t>N/A - not asscoiated with a Requirement</t>
   </si>
   <si>
-    <t>z</t>
-  </si>
-  <si>
     <t>SQA - Error found in TC296: SQA eBilling TAS US1 Test Case - Date of Onset Printed Regresstion Test 4 TS6</t>
   </si>
   <si>
@@ -137,19 +125,25 @@
   </si>
   <si>
     <t>CIT - Error found in TC363: CIT eBilling TAS US12 Print CMS Form/Replacement - TS11</t>
-  </si>
-  <si>
-    <t>IB*2.0*576T3</t>
-  </si>
-  <si>
-    <t>IB*2.0*576T5</t>
   </si>
   <si>
     <t>MCCF EDI TAS eBilling Build 1
 Defect Log</t>
   </si>
   <si>
-    <t>IB*2*576T6</t>
+    <t>IB*2.0*576 T3</t>
+  </si>
+  <si>
+    <t>IB*2.0*576 T4</t>
+  </si>
+  <si>
+    <t>IB*2.0*576 T5</t>
+  </si>
+  <si>
+    <t>IB*2.0*576 T6</t>
+  </si>
+  <si>
+    <t>IB*2*576 T6</t>
   </si>
 </sst>
 </file>
@@ -1255,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1278,7 +1272,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="15" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1339,13 +1333,13 @@
         <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -1357,10 +1351,10 @@
         <v>6</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>13</v>
@@ -1368,31 +1362,31 @@
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>13</v>
@@ -1400,13 +1394,13 @@
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -1415,16 +1409,16 @@
         <v>16</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>13</v>
@@ -1432,13 +1426,13 @@
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>11</v>
@@ -1447,16 +1441,16 @@
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>13</v>
@@ -1464,51 +1458,51 @@
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="16" customFormat="1" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>7</v>
@@ -1517,13 +1511,13 @@
         <v>6</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -1541,11 +1535,6 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J2"/>

</xml_diff>